<commit_message>
Adição das querys no código
</commit_message>
<xml_diff>
--- a/metas.xlsx
+++ b/metas.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">cdVendedor</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">cd_vendedor</t>
   </si>
   <si>
     <t xml:space="preserve">jan2017</t>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">dez2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,6 +226,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,13 +247,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Z12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.453125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.4453125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="1" style="1" width="13.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="13.43"/>
@@ -329,7 +336,9 @@
       <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0"/>
+      <c r="Z1" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
@@ -407,7 +416,10 @@
       <c r="Y2" s="6" t="n">
         <v>34296.9391405294</v>
       </c>
-      <c r="Z2" s="0"/>
+      <c r="Z2" s="7" t="n">
+        <f aca="false">SUM(B2:Y2)</f>
+        <v>3033854.44780951</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
@@ -485,7 +497,10 @@
       <c r="Y3" s="6" t="n">
         <v>46867.563533804</v>
       </c>
-      <c r="Z3" s="0"/>
+      <c r="Z3" s="7" t="n">
+        <f aca="false">SUM(B3:Y3)</f>
+        <v>2708056.70455845</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
@@ -563,7 +578,10 @@
       <c r="Y4" s="6" t="n">
         <v>32769.7730358222</v>
       </c>
-      <c r="Z4" s="0"/>
+      <c r="Z4" s="7" t="n">
+        <f aca="false">SUM(B4:Y4)</f>
+        <v>2050895.55737281</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
@@ -641,7 +659,10 @@
       <c r="Y5" s="6" t="n">
         <v>43339.5572587124</v>
       </c>
-      <c r="Z5" s="0"/>
+      <c r="Z5" s="7" t="n">
+        <f aca="false">SUM(B5:Y5)</f>
+        <v>427924.391967856</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
@@ -719,7 +740,10 @@
       <c r="Y6" s="6" t="n">
         <v>10380.6422106713</v>
       </c>
-      <c r="Z6" s="0"/>
+      <c r="Z6" s="6" t="n">
+        <f aca="false">SUM(B6:Y6)</f>
+        <v>2037216.81402516</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
@@ -797,7 +821,10 @@
       <c r="Y7" s="6" t="n">
         <v>92452.268238884</v>
       </c>
-      <c r="Z7" s="0"/>
+      <c r="Z7" s="6" t="n">
+        <f aca="false">SUM(B7:Y7)</f>
+        <v>5247942.73342008</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
@@ -875,7 +902,10 @@
       <c r="Y8" s="6" t="n">
         <v>41797.6707275318</v>
       </c>
-      <c r="Z8" s="0"/>
+      <c r="Z8" s="6" t="n">
+        <f aca="false">SUM(B8:Y8)</f>
+        <v>3830827.7604236</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
@@ -953,7 +983,10 @@
       <c r="Y9" s="6" t="n">
         <v>31620.1842535754</v>
       </c>
-      <c r="Z9" s="0"/>
+      <c r="Z9" s="6" t="n">
+        <f aca="false">SUM(B9:Y9)</f>
+        <v>1651439.50486814</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
@@ -1031,7 +1064,10 @@
       <c r="Y10" s="6" t="n">
         <v>56449.8759933361</v>
       </c>
-      <c r="Z10" s="0"/>
+      <c r="Z10" s="6" t="n">
+        <f aca="false">SUM(B10:Y10)</f>
+        <v>881940.536748293</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
@@ -1109,7 +1145,10 @@
       <c r="Y11" s="6" t="n">
         <v>18374.3462872232</v>
       </c>
-      <c r="Z11" s="0"/>
+      <c r="Z11" s="6" t="n">
+        <f aca="false">SUM(B11:Y11)</f>
+        <v>47213.3903379706</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
@@ -1187,7 +1226,10 @@
       <c r="Y12" s="6" t="n">
         <v>28028.7761468674</v>
       </c>
-      <c r="Z12" s="0"/>
+      <c r="Z12" s="6" t="n">
+        <f aca="false">SUM(B12:Y12)</f>
+        <v>1914090.38347007</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
@@ -1272,8 +1314,9 @@
       <c r="X15" s="0"/>
       <c r="Y15" s="0"/>
       <c r="Z15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA15" s="0"/>
+    </row>
+    <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
@@ -1299,9 +1342,8 @@
       <c r="W16" s="0"/>
       <c r="X16" s="0"/>
       <c r="Y16" s="0"/>
-      <c r="Z16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>
@@ -1327,8 +1369,25 @@
       <c r="W17" s="0"/>
       <c r="X17" s="0"/>
       <c r="Y17" s="0"/>
-      <c r="Z17" s="0"/>
-    </row>
+    </row>
+    <row r="18" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y18" s="0"/>
+    </row>
+    <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y19" s="0"/>
+    </row>
+    <row r="20" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y20" s="0"/>
+    </row>
+    <row r="21" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y21" s="0"/>
+    </row>
+    <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>